<commit_message>
fix: remover módulo de vendas e ajustar dashboard para total acumulado de receitas e despesas
</commit_message>
<xml_diff>
--- a/docs/Despesas.xlsx
+++ b/docs/Despesas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nandho\Financas\App_financeiro\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB0E37-A5AC-42B1-90D1-D66CFB1DCAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18838BAC-DA36-4C32-9331-39AFC9008D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7F73A568-E144-4E49-B461-0D267B4A4C55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3561" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="201">
   <si>
     <t>Alimentação</t>
   </si>
@@ -636,6 +636,9 @@
   </si>
   <si>
     <t>Mesada</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDF31777-EB8C-4C76-8E5A-79E50D5CB2EC}">
-  <dimension ref="A1:H594"/>
+  <dimension ref="A1:I594"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1029,7 @@
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -1051,8 +1054,11 @@
       <c r="H1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45659</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45659</v>
       </c>
@@ -1104,7 +1110,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45659</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45659</v>
       </c>
@@ -1156,7 +1162,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45659</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45659</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45659</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45659</v>
       </c>
@@ -1260,7 +1266,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45659</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45659</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45659</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45660</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45660</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45660</v>
       </c>
@@ -1416,7 +1422,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45660</v>
       </c>

</xml_diff>